<commit_message>
Added BJT data and lab images for MOSFET
</commit_message>
<xml_diff>
--- a/BJT/Data/data.xlsx
+++ b/BJT/Data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\3131\Projects\BJT\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F875FF6-CE0D-4363-89B5-3153EEC1D0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CDC929-42D1-4154-8C0F-8A4419327DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00A6F88C-B33A-4918-A874-9CDEED54ECDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00A6F88C-B33A-4918-A874-9CDEED54ECDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Theoretical</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>20.971M</t>
+  </si>
+  <si>
+    <t>111k</t>
   </si>
 </sst>
 </file>
@@ -125,7 +128,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -158,11 +161,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,7 +483,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,12 +508,12 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -562,7 +565,7 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="K4:N4" si="0">L4/M4</f>
+        <f t="shared" ref="N4" si="0">L4/M4</f>
         <v>0</v>
       </c>
     </row>
@@ -595,7 +598,7 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>1.853E-4</v>
       </c>
     </row>
@@ -603,7 +606,7 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>2.896E-2</v>
       </c>
     </row>
@@ -611,7 +614,7 @@
       <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>2.5060000000000002E-4</v>
       </c>
     </row>
@@ -619,24 +622,27 @@
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>6.5259999999999995E-5</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>231.6</v>
+      </c>
+      <c r="D12">
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -653,6 +659,9 @@
       </c>
       <c r="C14" t="s">
         <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
completed BJT measured data
</commit_message>
<xml_diff>
--- a/BJT/Data/data.xlsx
+++ b/BJT/Data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\3131\Projects\BJT\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CDC929-42D1-4154-8C0F-8A4419327DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67CEBF7-9639-4259-BE9F-6C1C2574F4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00A6F88C-B33A-4918-A874-9CDEED54ECDF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Theoretical</t>
   </si>
@@ -119,7 +119,46 @@
     <t>20.971M</t>
   </si>
   <si>
-    <t>111k</t>
+    <t>7.6k</t>
+  </si>
+  <si>
+    <t>9.7k</t>
+  </si>
+  <si>
+    <t>375K</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>3.108k</t>
+  </si>
+  <si>
+    <t>47.405k</t>
+  </si>
+  <si>
+    <t>RC</t>
+  </si>
+  <si>
+    <t>RE</t>
+  </si>
+  <si>
+    <t>9.439k</t>
+  </si>
+  <si>
+    <t>Swing Assymetry Voltage</t>
+  </si>
+  <si>
+    <t>80m</t>
+  </si>
+  <si>
+    <t>Ie</t>
   </si>
 </sst>
 </file>
@@ -159,13 +198,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,17 +520,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7316BDF1-41A5-4FD7-9ED5-82B815B0853F}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -522,6 +564,9 @@
       <c r="C3">
         <v>6.1550000000000002</v>
       </c>
+      <c r="D3">
+        <v>3.1240000000000001</v>
+      </c>
       <c r="H3" t="s">
         <v>17</v>
       </c>
@@ -548,25 +593,30 @@
       <c r="C4">
         <v>2.2189999999999999</v>
       </c>
+      <c r="D4">
+        <v>0.70399999999999996</v>
+      </c>
       <c r="H4">
-        <v>0</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <f>3.796*10^-6</f>
+        <v>3.7959999999999997E-6</v>
       </c>
       <c r="J4">
         <f>H4/I4</f>
-        <v>0</v>
+        <v>1580.6111696522657</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <f>33.468*10^-6</f>
+        <v>3.3467999999999999E-5</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4" si="0">L4/M4</f>
-        <v>0</v>
+        <v>2987.9287677781763</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -576,6 +626,9 @@
       <c r="C5">
         <v>1.4570000000000001</v>
       </c>
+      <c r="D5">
+        <v>2.8000000000000001E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -591,7 +644,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.0960000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -601,6 +654,9 @@
       <c r="C7" s="1">
         <v>1.853E-4</v>
       </c>
+      <c r="D7" s="4">
+        <v>2.8129499999999998E-4</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -609,101 +665,177 @@
       <c r="C8" s="1">
         <v>2.896E-2</v>
       </c>
+      <c r="D8" s="4">
+        <v>1.91E-3</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2.5060000000000002E-4</v>
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <f>SUM(C7,C8)</f>
+        <v>2.9145299999999999E-2</v>
+      </c>
+      <c r="D9" s="4">
+        <f>SUM(D7,D8)</f>
+        <v>2.1912950000000002E-3</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2.5060000000000002E-4</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2.8039999999999999E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>6.5259999999999995E-5</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="D11" s="4">
+        <v>2.6600700000000002E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="2">
-        <v>231.6</v>
-      </c>
-      <c r="D12">
-        <v>160</v>
-      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="C13" s="2">
+        <v>231.6</v>
+      </c>
+      <c r="D13">
+        <v>160</v>
+      </c>
+      <c r="L13" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>800</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>163.05000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>283</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C23">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C24">
         <f>47.2964-3</f>
         <v>44.296399999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C26">
-        <f>10^(C23/20)</f>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <f>10^(C24/20)</f>
         <v>163.99099465315723</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>164.83</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added data and images for BJT
</commit_message>
<xml_diff>
--- a/BJT/Data/data.xlsx
+++ b/BJT/Data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\3131\Projects\BJT\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B258351-8771-4B80-AEE3-70C38C5A177C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120139FD-5521-42D4-8511-3B74DA3319D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00A6F88C-B33A-4918-A874-9CDEED54ECDF}"/>
+    <workbookView xWindow="3675" yWindow="3645" windowWidth="21600" windowHeight="11295" xr2:uid="{00A6F88C-B33A-4918-A874-9CDEED54ECDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Theoretical</t>
   </si>
@@ -101,12 +101,6 @@
     <t>Iout</t>
   </si>
   <si>
-    <t>IR1</t>
-  </si>
-  <si>
-    <t>IR2</t>
-  </si>
-  <si>
     <t>Max Gain</t>
   </si>
   <si>
@@ -122,12 +116,6 @@
     <t>7.6k</t>
   </si>
   <si>
-    <t>9.7k</t>
-  </si>
-  <si>
-    <t>375K</t>
-  </si>
-  <si>
     <t>`</t>
   </si>
   <si>
@@ -159,6 +147,21 @@
   </si>
   <si>
     <t>Ie</t>
+  </si>
+  <si>
+    <t>5.1k</t>
+  </si>
+  <si>
+    <t>9.9k</t>
+  </si>
+  <si>
+    <t>480k</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Frequency Bandwidth</t>
   </si>
 </sst>
 </file>
@@ -522,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7316BDF1-41A5-4FD7-9ED5-82B815B0853F}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,6 +551,9 @@
       <c r="D1" t="s">
         <v>15</v>
       </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -565,7 +571,11 @@
         <v>6.1550000000000002</v>
       </c>
       <c r="D3">
-        <v>3.1240000000000001</v>
+        <v>7.6</v>
+      </c>
+      <c r="E3">
+        <f>ABS(C3-D3)/C3</f>
+        <v>0.2347684809098293</v>
       </c>
       <c r="H3" t="s">
         <v>17</v>
@@ -594,7 +604,11 @@
         <v>2.2189999999999999</v>
       </c>
       <c r="D4">
-        <v>0.70399999999999996</v>
+        <v>2.0720000000000001</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E11" si="0">ABS(C4-D4)/C4</f>
+        <v>6.6246056782334292E-2</v>
       </c>
       <c r="H4">
         <v>6.0000000000000001E-3</v>
@@ -615,7 +629,7 @@
         <v>3.3467999999999999E-5</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4" si="0">L4/M4</f>
+        <f t="shared" ref="N4" si="1">L4/M4</f>
         <v>2987.9287677781763</v>
       </c>
     </row>
@@ -627,7 +641,11 @@
         <v>1.4570000000000001</v>
       </c>
       <c r="D5">
-        <v>2.8000000000000001E-2</v>
+        <v>1.4650000000000001</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>5.4907343857240956E-3</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -639,12 +657,16 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:D6" si="1">C3-C5</f>
+        <f t="shared" ref="C6:D6" si="2">C3-C5</f>
         <v>4.6980000000000004</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
-        <v>3.0960000000000001</v>
+        <f t="shared" si="2"/>
+        <v>6.1349999999999998</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.30587484035759882</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -655,7 +677,12 @@
         <v>1.853E-4</v>
       </c>
       <c r="D7" s="3">
-        <v>2.8129499999999998E-4</v>
+        <f>14.12*10^-6</f>
+        <v>1.4119999999999999E-5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.92379924446842954</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -666,12 +693,16 @@
         <v>2.896E-2</v>
       </c>
       <c r="D8" s="3">
-        <v>1.91E-3</v>
+        <v>2.8700000000000002E-3</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.90089779005524862</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C9">
         <f>SUM(C7,C8)</f>
@@ -679,30 +710,20 @@
       </c>
       <c r="D9" s="3">
         <f>SUM(D7,D8)</f>
-        <v>2.1912950000000002E-3</v>
+        <v>2.88412E-3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.90104339293127877</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2.5060000000000002E-4</v>
-      </c>
-      <c r="D10" s="3">
-        <v>2.8039999999999999E-4</v>
-      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1">
-        <v>6.5259999999999995E-5</v>
-      </c>
-      <c r="D11" s="3">
-        <v>2.6600700000000002E-4</v>
-      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -714,16 +735,16 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2">
         <v>231.6</v>
       </c>
       <c r="D13">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="L13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -731,10 +752,10 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14">
-        <v>800</v>
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -742,10 +763,10 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -753,10 +774,10 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -781,17 +802,30 @@
         <v>2987.9287677781763</v>
       </c>
     </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19">
+        <f>20971-1.22</f>
+        <v>20969.78</v>
+      </c>
+      <c r="D19">
+        <f>480-5.1</f>
+        <v>474.9</v>
+      </c>
+    </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -808,31 +842,31 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B38">
         <v>164.83</v>

</xml_diff>

<commit_message>
Added BJT Hand calculations
</commit_message>
<xml_diff>
--- a/BJT/Data/data.xlsx
+++ b/BJT/Data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\3131\Projects\BJT\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42FDF27-9531-4B71-B8FC-640F92410679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408CAC8B-C370-4558-8EFB-09B3BD1AF19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00A6F88C-B33A-4918-A874-9CDEED54ECDF}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00A6F88C-B33A-4918-A874-9CDEED54ECDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,6 +567,9 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>6.0469999999999997</v>
+      </c>
       <c r="C3">
         <v>6.1550000000000002</v>
       </c>
@@ -600,6 +603,9 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>2.214</v>
+      </c>
       <c r="C4">
         <v>2.2189999999999999</v>
       </c>
@@ -607,7 +613,7 @@
         <v>2.0720000000000001</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E11" si="0">ABS(C4-D4)/C4</f>
+        <f t="shared" ref="E4:E9" si="0">ABS(C4-D4)/C4</f>
         <v>6.6246056782334292E-2</v>
       </c>
       <c r="H4">
@@ -637,6 +643,9 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>1.514</v>
+      </c>
       <c r="C5">
         <v>1.4570000000000001</v>
       </c>
@@ -654,7 +663,7 @@
       </c>
       <c r="B6">
         <f>B3-B5</f>
-        <v>0</v>
+        <v>4.5329999999999995</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:D6" si="2">C3-C5</f>
@@ -673,6 +682,10 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7">
+        <f>186*10^-6</f>
+        <v>1.8599999999999999E-4</v>
+      </c>
       <c r="C7" s="1">
         <v>1.853E-4</v>
       </c>
@@ -689,6 +702,9 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>2.9100000000000001E-2</v>
+      </c>
       <c r="C8" s="1">
         <v>2.896E-2</v>
       </c>
@@ -704,6 +720,9 @@
       <c r="A9" t="s">
         <v>36</v>
       </c>
+      <c r="B9">
+        <v>2.93E-2</v>
+      </c>
       <c r="C9">
         <f>SUM(C7,C8)</f>
         <v>2.9145299999999999E-2</v>
@@ -737,6 +756,9 @@
       <c r="A13" t="s">
         <v>21</v>
       </c>
+      <c r="B13">
+        <v>282.76</v>
+      </c>
       <c r="C13" s="2">
         <v>231.6</v>
       </c>
@@ -784,6 +806,9 @@
       <c r="A17" t="s">
         <v>13</v>
       </c>
+      <c r="B17">
+        <v>157.017</v>
+      </c>
       <c r="C17">
         <v>163.05000000000001</v>
       </c>
@@ -794,6 +819,9 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
+      </c>
+      <c r="B18">
+        <v>318.35000000000002</v>
       </c>
       <c r="C18">
         <v>283</v>

</xml_diff>